<commit_message>
ploting the finance minister and nepse index with sector index
</commit_message>
<xml_diff>
--- a/stock/data/finance/2077asoj28.xlsx
+++ b/stock/data/finance/2077asoj28.xlsx
@@ -185,7 +185,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -203,15 +203,30 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf fontId="2" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf fontId="2" fillId="3" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf fontId="2" fillId="3" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf fontId="2" fillId="3" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf fontId="2" fillId="0" borderId="1" numFmtId="164" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="2" fillId="0" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="2" fillId="0" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="2" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="2" fillId="3" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -220,16 +235,7 @@
     <xf fontId="2" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf fontId="2" fillId="0" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf fontId="2" fillId="3" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf fontId="2" fillId="3" borderId="3" numFmtId="165" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf fontId="2" fillId="0" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf fontId="2" fillId="0" borderId="3" numFmtId="165" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -733,7 +739,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -796,851 +802,1901 @@
     </row>
     <row r="2" ht="14.25">
       <c r="A2" s="5">
-        <v>44122</v>
+        <v>44091</v>
       </c>
       <c r="B2" s="6">
-        <v>1243.0021999999999</v>
+        <v>1249.3776</v>
       </c>
       <c r="C2" s="7">
-        <v>1730.0260000000001</v>
-      </c>
-      <c r="D2" s="6">
-        <v>1011.7074</v>
-      </c>
-      <c r="E2" s="6">
-        <v>1326.0165999999999</v>
+        <v>1884.5418</v>
+      </c>
+      <c r="D2" s="8">
+        <v>1020.6917</v>
+      </c>
+      <c r="E2" s="8">
+        <v>1290.0549000000001</v>
       </c>
       <c r="F2" s="7">
-        <v>2027.3876</v>
-      </c>
-      <c r="G2" s="8">
-        <v>3002.0704999999998</v>
-      </c>
-      <c r="H2" s="6">
-        <v>2504.6623</v>
-      </c>
-      <c r="I2" s="6">
-        <v>9423.2183000000005</v>
+        <v>1837.9621999999999</v>
+      </c>
+      <c r="G2" s="7">
+        <v>3066.1788999999999</v>
+      </c>
+      <c r="H2" s="7">
+        <v>312.50200000000001</v>
+      </c>
+      <c r="I2" s="8">
+        <v>1572.1855</v>
       </c>
       <c r="J2" s="7">
-        <v>7735.7745999999997</v>
-      </c>
-      <c r="K2" s="8">
-        <v>820.0385</v>
-      </c>
-      <c r="L2" s="8">
-        <v>1065.23</v>
-      </c>
-      <c r="M2" s="6">
-        <v>108.2895</v>
-      </c>
-      <c r="N2" s="6">
-        <v>101.7206</v>
-      </c>
-      <c r="O2" s="7">
-        <v>308.2792</v>
-      </c>
-      <c r="P2" s="6">
-        <v>1556.8027999999999</v>
+        <v>8147.4795000000004</v>
+      </c>
+      <c r="K2" s="7">
+        <v>726.85749999999996</v>
+      </c>
+      <c r="L2" s="7">
+        <v>1016.8316</v>
+      </c>
+      <c r="M2" s="8">
+        <v>108.82259999999999</v>
+      </c>
+      <c r="N2" s="8">
+        <v>2605.4629</v>
+      </c>
+      <c r="O2" s="8">
+        <v>102.5797</v>
+      </c>
+      <c r="P2" s="8">
+        <v>9879.9555</v>
       </c>
     </row>
     <row r="3" ht="14.25">
       <c r="A3" s="9">
-        <v>44123</v>
+        <v>44094</v>
       </c>
       <c r="B3" s="10">
-        <v>1250.6735000000001</v>
+        <v>1268.7925</v>
       </c>
       <c r="C3" s="11">
-        <v>1744.1883</v>
-      </c>
-      <c r="D3" s="10">
-        <v>1019.3059</v>
-      </c>
-      <c r="E3" s="10">
-        <v>1369.8780999999999</v>
+        <v>1787.8870999999999</v>
+      </c>
+      <c r="D3" s="12">
+        <v>1010.335</v>
+      </c>
+      <c r="E3" s="12">
+        <v>1237.6815999999999</v>
       </c>
       <c r="F3" s="11">
-        <v>2057.8168000000001</v>
-      </c>
-      <c r="G3" s="12">
-        <v>3009.2399999999998</v>
-      </c>
-      <c r="H3" s="10">
-        <v>2515.3027000000002</v>
-      </c>
-      <c r="I3" s="10">
-        <v>9473.8101000000006</v>
+        <v>1863.8467000000001</v>
+      </c>
+      <c r="G3" s="11">
+        <v>3064.0104000000001</v>
+      </c>
+      <c r="H3" s="11">
+        <v>313.6207</v>
+      </c>
+      <c r="I3" s="12">
+        <v>1575.1838</v>
       </c>
       <c r="J3" s="11">
-        <v>7835.2954</v>
-      </c>
-      <c r="K3" s="12">
-        <v>836.29459999999995</v>
-      </c>
-      <c r="L3" s="12">
-        <v>1063.5404000000001</v>
-      </c>
-      <c r="M3" s="10">
-        <v>109.42100000000001</v>
-      </c>
-      <c r="N3" s="10">
-        <v>102.6147</v>
-      </c>
-      <c r="O3" s="11">
-        <v>310.89850000000001</v>
-      </c>
-      <c r="P3" s="10">
-        <v>1570.3838000000001</v>
+        <v>8077.3698999999997</v>
+      </c>
+      <c r="K3" s="11">
+        <v>755.51300000000003</v>
+      </c>
+      <c r="L3" s="11">
+        <v>1016.8316</v>
+      </c>
+      <c r="M3" s="12">
+        <v>109.2932</v>
+      </c>
+      <c r="N3" s="12">
+        <v>2591.6541000000002</v>
+      </c>
+      <c r="O3" s="12">
+        <v>103.1409</v>
+      </c>
+      <c r="P3" s="12">
+        <v>9823.6988999999994</v>
       </c>
     </row>
     <row r="4" ht="14.25">
       <c r="A4" s="5">
-        <v>44124</v>
+        <v>44095</v>
       </c>
       <c r="B4" s="6">
-        <v>1258.4109000000001</v>
+        <v>1264.4715000000001</v>
       </c>
       <c r="C4" s="7">
-        <v>1763.454</v>
-      </c>
-      <c r="D4" s="6">
-        <v>1030.7067999999999</v>
-      </c>
-      <c r="E4" s="6">
-        <v>1399.8406</v>
+        <v>1755.2802999999999</v>
+      </c>
+      <c r="D4" s="8">
+        <v>1008.9083000000001</v>
+      </c>
+      <c r="E4" s="8">
+        <v>1231.8059000000001</v>
       </c>
       <c r="F4" s="7">
-        <v>2080.0038</v>
-      </c>
-      <c r="G4" s="8">
-        <v>3034.6017000000002</v>
-      </c>
-      <c r="H4" s="6">
-        <v>2531.7451999999998</v>
-      </c>
-      <c r="I4" s="6">
-        <v>9551.9256999999998</v>
+        <v>1852.3418999999999</v>
+      </c>
+      <c r="G4" s="7">
+        <v>3076.2411999999999</v>
+      </c>
+      <c r="H4" s="7">
+        <v>312.24349999999998</v>
+      </c>
+      <c r="I4" s="8">
+        <v>1569.0648000000001</v>
       </c>
       <c r="J4" s="7">
-        <v>7891.0528999999997</v>
-      </c>
-      <c r="K4" s="8">
-        <v>844.89269999999999</v>
-      </c>
-      <c r="L4" s="8">
-        <v>1066.4971</v>
-      </c>
-      <c r="M4" s="6">
-        <v>110.3143</v>
-      </c>
-      <c r="N4" s="6">
-        <v>103.432</v>
-      </c>
-      <c r="O4" s="7">
-        <v>313.55270000000002</v>
-      </c>
-      <c r="P4" s="6">
-        <v>1583.7799</v>
+        <v>8022.3876</v>
+      </c>
+      <c r="K4" s="7">
+        <v>746.07870000000003</v>
+      </c>
+      <c r="L4" s="7">
+        <v>1005.8404</v>
+      </c>
+      <c r="M4" s="8">
+        <v>108.9222</v>
+      </c>
+      <c r="N4" s="8">
+        <v>2584.2748000000001</v>
+      </c>
+      <c r="O4" s="8">
+        <v>102.708</v>
+      </c>
+      <c r="P4" s="8">
+        <v>9755.8528000000006</v>
       </c>
     </row>
     <row r="5" ht="14.25">
       <c r="A5" s="9">
-        <v>44125</v>
+        <v>44096</v>
       </c>
       <c r="B5" s="10">
-        <v>1279.9563000000001</v>
+        <v>1242.1089999999999</v>
       </c>
       <c r="C5" s="11">
-        <v>1748.4223999999999</v>
-      </c>
-      <c r="D5" s="10">
-        <v>1033.752</v>
-      </c>
-      <c r="E5" s="10">
-        <v>1385.7536</v>
+        <v>1740.2166</v>
+      </c>
+      <c r="D5" s="12">
+        <v>1001.684</v>
+      </c>
+      <c r="E5" s="12">
+        <v>1206.8941</v>
       </c>
       <c r="F5" s="11">
-        <v>2090.0391</v>
-      </c>
-      <c r="G5" s="12">
-        <v>3028.2721999999999</v>
-      </c>
-      <c r="H5" s="10">
-        <v>2535.1552000000001</v>
-      </c>
-      <c r="I5" s="10">
-        <v>9609.8682000000008</v>
+        <v>1811.1803</v>
+      </c>
+      <c r="G5" s="11">
+        <v>3041.1984000000002</v>
+      </c>
+      <c r="H5" s="11">
+        <v>307.39949999999999</v>
+      </c>
+      <c r="I5" s="12">
+        <v>1546.1585</v>
       </c>
       <c r="J5" s="11">
-        <v>7955.3289999999997</v>
-      </c>
-      <c r="K5" s="12">
-        <v>844.29160000000002</v>
-      </c>
-      <c r="L5" s="12">
-        <v>1089.8939</v>
-      </c>
-      <c r="M5" s="10">
-        <v>111.48099999999999</v>
-      </c>
-      <c r="N5" s="10">
-        <v>104.7525</v>
-      </c>
-      <c r="O5" s="11">
-        <v>316.65140000000002</v>
-      </c>
-      <c r="P5" s="10">
-        <v>1597.7149999999999</v>
+        <v>7909.7313999999997</v>
+      </c>
+      <c r="K5" s="11">
+        <v>733.58799999999997</v>
+      </c>
+      <c r="L5" s="11">
+        <v>1012.9456</v>
+      </c>
+      <c r="M5" s="12">
+        <v>107.16930000000001</v>
+      </c>
+      <c r="N5" s="12">
+        <v>2561.0315999999998</v>
+      </c>
+      <c r="O5" s="12">
+        <v>100.9928</v>
+      </c>
+      <c r="P5" s="12">
+        <v>9646.3801999999996</v>
       </c>
     </row>
     <row r="6" ht="14.25">
       <c r="A6" s="5">
-        <v>44126</v>
+        <v>44097</v>
       </c>
       <c r="B6" s="6">
-        <v>1292.0539000000001</v>
+        <v>1243.9776999999999</v>
       </c>
       <c r="C6" s="7">
-        <v>1734.3866</v>
-      </c>
-      <c r="D6" s="6">
-        <v>1039.0261</v>
-      </c>
-      <c r="E6" s="6">
-        <v>1379.3216</v>
+        <v>1716.5743</v>
+      </c>
+      <c r="D6" s="8">
+        <v>1009.0473</v>
+      </c>
+      <c r="E6" s="8">
+        <v>1240.6883</v>
       </c>
       <c r="F6" s="7">
-        <v>2091.7447999999999</v>
-      </c>
-      <c r="G6" s="8">
-        <v>3057.7514000000001</v>
-      </c>
-      <c r="H6" s="6">
-        <v>2535.9612000000002</v>
-      </c>
-      <c r="I6" s="6">
-        <v>9599.7705000000005</v>
+        <v>1833.9826</v>
+      </c>
+      <c r="G6" s="7">
+        <v>3064.3955999999998</v>
+      </c>
+      <c r="H6" s="7">
+        <v>308.34769999999997</v>
+      </c>
+      <c r="I6" s="8">
+        <v>1555.5274999999999</v>
       </c>
       <c r="J6" s="7">
-        <v>7993.8486999999996</v>
-      </c>
-      <c r="K6" s="8">
-        <v>849.67520000000002</v>
-      </c>
-      <c r="L6" s="8">
-        <v>1099.2276999999999</v>
-      </c>
-      <c r="M6" s="6">
-        <v>112.0997</v>
-      </c>
-      <c r="N6" s="6">
-        <v>105.3152</v>
-      </c>
-      <c r="O6" s="7">
-        <v>318.56229999999999</v>
-      </c>
-      <c r="P6" s="6">
-        <v>1606.2552000000001</v>
+        <v>7984.5045</v>
+      </c>
+      <c r="K6" s="7">
+        <v>745.60559999999998</v>
+      </c>
+      <c r="L6" s="7">
+        <v>1018.6679</v>
+      </c>
+      <c r="M6" s="8">
+        <v>107.82859999999999</v>
+      </c>
+      <c r="N6" s="8">
+        <v>2571.2511</v>
+      </c>
+      <c r="O6" s="8">
+        <v>101.3717</v>
+      </c>
+      <c r="P6" s="8">
+        <v>9741.0558000000001</v>
       </c>
     </row>
     <row r="7" ht="14.25">
       <c r="A7" s="9">
-        <v>44132</v>
+        <v>44098</v>
       </c>
       <c r="B7" s="10">
-        <v>1347.2005999999999</v>
+        <v>1244.9054000000001</v>
       </c>
       <c r="C7" s="11">
-        <v>1767.2349999999999</v>
-      </c>
-      <c r="D7" s="10">
-        <v>1053.5986</v>
-      </c>
-      <c r="E7" s="10">
-        <v>1383.1831999999999</v>
+        <v>1733.8438000000001</v>
+      </c>
+      <c r="D7" s="12">
+        <v>1017.9874</v>
+      </c>
+      <c r="E7" s="12">
+        <v>1296.396</v>
       </c>
       <c r="F7" s="11">
-        <v>2152.7168000000001</v>
-      </c>
-      <c r="G7" s="12">
-        <v>3078.6302999999998</v>
-      </c>
-      <c r="H7" s="10">
-        <v>2561.152</v>
-      </c>
-      <c r="I7" s="10">
-        <v>9710.4493000000002</v>
+        <v>1832.3136999999999</v>
+      </c>
+      <c r="G7" s="11">
+        <v>3055.098</v>
+      </c>
+      <c r="H7" s="11">
+        <v>309.57279999999997</v>
+      </c>
+      <c r="I7" s="12">
+        <v>1561.2701999999999</v>
       </c>
       <c r="J7" s="11">
-        <v>8040.9139999999998</v>
-      </c>
-      <c r="K7" s="12">
-        <v>863.05719999999997</v>
-      </c>
-      <c r="L7" s="12">
-        <v>1090.4014</v>
-      </c>
-      <c r="M7" s="10">
-        <v>115.3723</v>
-      </c>
-      <c r="N7" s="10">
-        <v>108.6108</v>
-      </c>
-      <c r="O7" s="11">
-        <v>327.76859999999999</v>
-      </c>
-      <c r="P7" s="10">
-        <v>1647.4595999999999</v>
+        <v>7930.5366999999997</v>
+      </c>
+      <c r="K7" s="11">
+        <v>755.22140000000002</v>
+      </c>
+      <c r="L7" s="11">
+        <v>1089.5137</v>
+      </c>
+      <c r="M7" s="12">
+        <v>108.22669999999999</v>
+      </c>
+      <c r="N7" s="12">
+        <v>2570.7314000000001</v>
+      </c>
+      <c r="O7" s="12">
+        <v>101.6827</v>
+      </c>
+      <c r="P7" s="12">
+        <v>9696.9549000000006</v>
       </c>
     </row>
     <row r="8" ht="14.25">
       <c r="A8" s="5">
-        <v>44133</v>
+        <v>44101</v>
       </c>
       <c r="B8" s="6">
-        <v>1340.9271000000001</v>
+        <v>1258.6474000000001</v>
       </c>
       <c r="C8" s="7">
-        <v>1751.8191999999999</v>
-      </c>
-      <c r="D8" s="6">
-        <v>1059.4296999999999</v>
-      </c>
-      <c r="E8" s="6">
-        <v>1389.9331</v>
+        <v>1785.5530000000001</v>
+      </c>
+      <c r="D8" s="8">
+        <v>1016.4447</v>
+      </c>
+      <c r="E8" s="8">
+        <v>1283.2985000000001</v>
       </c>
       <c r="F8" s="7">
-        <v>2135.8955999999998</v>
-      </c>
-      <c r="G8" s="8">
-        <v>3043.7838000000002</v>
-      </c>
-      <c r="H8" s="6">
-        <v>2573.8876</v>
-      </c>
-      <c r="I8" s="6">
-        <v>9719.3099999999995</v>
+        <v>1845.3114</v>
+      </c>
+      <c r="G8" s="7">
+        <v>3010.2918</v>
+      </c>
+      <c r="H8" s="7">
+        <v>310.47620000000001</v>
+      </c>
+      <c r="I8" s="8">
+        <v>1565.5559000000001</v>
       </c>
       <c r="J8" s="7">
-        <v>8080.8068999999996</v>
-      </c>
-      <c r="K8" s="8">
-        <v>860.43230000000005</v>
-      </c>
-      <c r="L8" s="8">
-        <v>1105.3524</v>
-      </c>
-      <c r="M8" s="6">
-        <v>115.1695</v>
-      </c>
-      <c r="N8" s="6">
-        <v>108.5177</v>
-      </c>
-      <c r="O8" s="7">
-        <v>328.04239999999999</v>
-      </c>
-      <c r="P8" s="6">
-        <v>1645.6790000000001</v>
+        <v>7858.0021999999999</v>
+      </c>
+      <c r="K8" s="7">
+        <v>767.15409999999997</v>
+      </c>
+      <c r="L8" s="7">
+        <v>1087.5707</v>
+      </c>
+      <c r="M8" s="8">
+        <v>108.71169999999999</v>
+      </c>
+      <c r="N8" s="8">
+        <v>2564.1100000000001</v>
+      </c>
+      <c r="O8" s="8">
+        <v>102.1733</v>
+      </c>
+      <c r="P8" s="8">
+        <v>9613.3628000000008</v>
       </c>
     </row>
     <row r="9" ht="14.25">
       <c r="A9" s="9">
-        <v>44136</v>
+        <v>44102</v>
       </c>
       <c r="B9" s="10">
-        <v>1326.3777</v>
+        <v>1254.6185</v>
       </c>
       <c r="C9" s="11">
-        <v>1736.53</v>
-      </c>
-      <c r="D9" s="10">
-        <v>1064.7896000000001</v>
-      </c>
-      <c r="E9" s="10">
-        <v>1409.2402999999999</v>
+        <v>1766.1608000000001</v>
+      </c>
+      <c r="D9" s="12">
+        <v>1016.3402</v>
+      </c>
+      <c r="E9" s="12">
+        <v>1280.3871999999999</v>
       </c>
       <c r="F9" s="11">
-        <v>2128.9187999999999</v>
-      </c>
-      <c r="G9" s="12">
-        <v>3028.5708</v>
-      </c>
-      <c r="H9" s="10">
-        <v>2603.2926000000002</v>
-      </c>
-      <c r="I9" s="10">
-        <v>9711.8593000000001</v>
+        <v>1847.5489</v>
+      </c>
+      <c r="G9" s="11">
+        <v>2990.6482000000001</v>
+      </c>
+      <c r="H9" s="11">
+        <v>309.60660000000001</v>
+      </c>
+      <c r="I9" s="12">
+        <v>1560.8308</v>
       </c>
       <c r="J9" s="11">
-        <v>8091.2551000000003</v>
-      </c>
-      <c r="K9" s="12">
-        <v>858.25580000000002</v>
-      </c>
-      <c r="L9" s="12">
-        <v>1129.7229</v>
-      </c>
-      <c r="M9" s="10">
-        <v>114.7953</v>
-      </c>
-      <c r="N9" s="10">
-        <v>107.907</v>
-      </c>
-      <c r="O9" s="11">
-        <v>326.63279999999997</v>
-      </c>
-      <c r="P9" s="10">
-        <v>1640.9593</v>
+        <v>7808.1732000000002</v>
+      </c>
+      <c r="K9" s="11">
+        <v>778.56259999999997</v>
+      </c>
+      <c r="L9" s="11">
+        <v>1072.8841</v>
+      </c>
+      <c r="M9" s="12">
+        <v>108.4054</v>
+      </c>
+      <c r="N9" s="12">
+        <v>2556.4973</v>
+      </c>
+      <c r="O9" s="12">
+        <v>101.83199999999999</v>
+      </c>
+      <c r="P9" s="12">
+        <v>9560.4577000000008</v>
       </c>
     </row>
     <row r="10" ht="14.25">
       <c r="A10" s="5">
-        <v>44137</v>
+        <v>44103</v>
       </c>
       <c r="B10" s="6">
-        <v>1314.7537</v>
+        <v>1243.7937999999999</v>
       </c>
       <c r="C10" s="7">
-        <v>1745.8626999999999</v>
-      </c>
-      <c r="D10" s="6">
-        <v>1061.5012999999999</v>
-      </c>
-      <c r="E10" s="6">
-        <v>1409.7791999999999</v>
+        <v>1756.0853999999999</v>
+      </c>
+      <c r="D10" s="8">
+        <v>1011.4009</v>
+      </c>
+      <c r="E10" s="8">
+        <v>1308.4341999999999</v>
       </c>
       <c r="F10" s="7">
-        <v>2128.6161999999999</v>
-      </c>
-      <c r="G10" s="8">
-        <v>3032.4544000000001</v>
-      </c>
-      <c r="H10" s="6">
-        <v>2665.5909000000001</v>
-      </c>
-      <c r="I10" s="6">
-        <v>9702.4599999999991</v>
+        <v>1846.8735999999999</v>
+      </c>
+      <c r="G10" s="7">
+        <v>2996.6466</v>
+      </c>
+      <c r="H10" s="7">
+        <v>307.82119999999998</v>
+      </c>
+      <c r="I10" s="8">
+        <v>1553.624</v>
       </c>
       <c r="J10" s="7">
-        <v>8118.5070999999998</v>
-      </c>
-      <c r="K10" s="8">
-        <v>862.21140000000003</v>
-      </c>
-      <c r="L10" s="8">
-        <v>1164.24</v>
-      </c>
-      <c r="M10" s="6">
-        <v>114.4892</v>
-      </c>
-      <c r="N10" s="6">
-        <v>107.5675</v>
-      </c>
-      <c r="O10" s="7">
-        <v>325.46409999999997</v>
-      </c>
-      <c r="P10" s="6">
-        <v>1637.6311000000001</v>
+        <v>7763.1858000000002</v>
+      </c>
+      <c r="K10" s="7">
+        <v>775.51670000000001</v>
+      </c>
+      <c r="L10" s="7">
+        <v>1048.8853999999999</v>
+      </c>
+      <c r="M10" s="8">
+        <v>107.8693</v>
+      </c>
+      <c r="N10" s="8">
+        <v>2542.9198999999999</v>
+      </c>
+      <c r="O10" s="8">
+        <v>101.20529999999999</v>
+      </c>
+      <c r="P10" s="8">
+        <v>9517.5013999999992</v>
       </c>
     </row>
     <row r="11" ht="14.25">
       <c r="A11" s="9">
-        <v>44138</v>
+        <v>44104</v>
       </c>
       <c r="B11" s="10">
-        <v>1312.5835999999999</v>
+        <v>1239.6199999999999</v>
       </c>
       <c r="C11" s="11">
-        <v>1747.8268</v>
-      </c>
-      <c r="D11" s="10">
-        <v>1076.3024</v>
-      </c>
-      <c r="E11" s="10">
-        <v>1416.921</v>
+        <v>1741.0859</v>
+      </c>
+      <c r="D11" s="12">
+        <v>1008.645</v>
+      </c>
+      <c r="E11" s="12">
+        <v>1317.1367</v>
       </c>
       <c r="F11" s="11">
-        <v>2112.4022</v>
-      </c>
-      <c r="G11" s="12">
-        <v>3038.4056999999998</v>
-      </c>
-      <c r="H11" s="10">
-        <v>2672.4218000000001</v>
-      </c>
-      <c r="I11" s="10">
-        <v>9716.4567999999999</v>
+        <v>1881.4184</v>
+      </c>
+      <c r="G11" s="11">
+        <v>2989.4294</v>
+      </c>
+      <c r="H11" s="11">
+        <v>307.17829999999998</v>
+      </c>
+      <c r="I11" s="12">
+        <v>1550.4348</v>
       </c>
       <c r="J11" s="11">
-        <v>8295.3667999999998</v>
-      </c>
-      <c r="K11" s="12">
-        <v>867.60789999999997</v>
-      </c>
-      <c r="L11" s="12">
-        <v>1220.1588999999999</v>
-      </c>
-      <c r="M11" s="10">
-        <v>114.5771</v>
-      </c>
-      <c r="N11" s="10">
-        <v>107.5385</v>
-      </c>
-      <c r="O11" s="11">
-        <v>326.6044</v>
-      </c>
-      <c r="P11" s="10">
-        <v>1643.0351000000001</v>
+        <v>7711.6329999999998</v>
+      </c>
+      <c r="K11" s="11">
+        <v>778.52359999999999</v>
+      </c>
+      <c r="L11" s="11">
+        <v>1037.7992999999999</v>
+      </c>
+      <c r="M11" s="12">
+        <v>107.69029999999999</v>
+      </c>
+      <c r="N11" s="12">
+        <v>2536.0493999999999</v>
+      </c>
+      <c r="O11" s="12">
+        <v>100.9988</v>
+      </c>
+      <c r="P11" s="12">
+        <v>9481.8060999999998</v>
       </c>
     </row>
     <row r="12" ht="14.25">
       <c r="A12" s="5">
-        <v>44139</v>
+        <v>44105</v>
       </c>
       <c r="B12" s="6">
-        <v>1309.5478000000001</v>
+        <v>1258.4804999999999</v>
       </c>
       <c r="C12" s="7">
-        <v>1752.4931999999999</v>
-      </c>
-      <c r="D12" s="6">
-        <v>1081.6943000000001</v>
-      </c>
-      <c r="E12" s="6">
-        <v>1418.5012999999999</v>
+        <v>1749.1650999999999</v>
+      </c>
+      <c r="D12" s="8">
+        <v>1011.6109</v>
+      </c>
+      <c r="E12" s="8">
+        <v>1292.3802000000001</v>
       </c>
       <c r="F12" s="7">
-        <v>2100.9791</v>
-      </c>
-      <c r="G12" s="8">
-        <v>3038.2975000000001</v>
-      </c>
-      <c r="H12" s="6">
-        <v>2668.759</v>
-      </c>
-      <c r="I12" s="6">
-        <v>9703.7829999999994</v>
+        <v>1946.8969</v>
+      </c>
+      <c r="G12" s="7">
+        <v>3039.982</v>
+      </c>
+      <c r="H12" s="7">
+        <v>310.15929999999997</v>
+      </c>
+      <c r="I12" s="8">
+        <v>1571.0434</v>
       </c>
       <c r="J12" s="7">
-        <v>8206.6826000000001</v>
-      </c>
-      <c r="K12" s="8">
-        <v>864.72490000000005</v>
-      </c>
-      <c r="L12" s="8">
-        <v>1245.4697000000001</v>
-      </c>
-      <c r="M12" s="6">
-        <v>114.35899999999999</v>
-      </c>
-      <c r="N12" s="6">
-        <v>107.34820000000001</v>
-      </c>
-      <c r="O12" s="7">
-        <v>326.49790000000002</v>
-      </c>
-      <c r="P12" s="6">
-        <v>1640.6425999999999</v>
+        <v>8044.0461999999998</v>
+      </c>
+      <c r="K12" s="7">
+        <v>784.31150000000002</v>
+      </c>
+      <c r="L12" s="7">
+        <v>1057.3320000000001</v>
+      </c>
+      <c r="M12" s="8">
+        <v>109.2456</v>
+      </c>
+      <c r="N12" s="8">
+        <v>2556.8631</v>
+      </c>
+      <c r="O12" s="8">
+        <v>102.25239999999999</v>
+      </c>
+      <c r="P12" s="8">
+        <v>9639.1358</v>
       </c>
     </row>
     <row r="13" ht="14.25">
       <c r="A13" s="9">
-        <v>44140</v>
+        <v>44108</v>
       </c>
       <c r="B13" s="10">
-        <v>1301.5358000000001</v>
+        <v>1274.0418999999999</v>
       </c>
       <c r="C13" s="11">
-        <v>1757.3549</v>
-      </c>
-      <c r="D13" s="10">
-        <v>1080.8372999999999</v>
-      </c>
-      <c r="E13" s="10">
-        <v>1432.4299000000001</v>
+        <v>1761.0300999999999</v>
+      </c>
+      <c r="D13" s="12">
+        <v>1022.7643</v>
+      </c>
+      <c r="E13" s="12">
+        <v>1277.1203</v>
       </c>
       <c r="F13" s="11">
-        <v>2106.0338000000002</v>
-      </c>
-      <c r="G13" s="12">
-        <v>3034.0862999999999</v>
-      </c>
-      <c r="H13" s="10">
-        <v>2655.4198999999999</v>
-      </c>
-      <c r="I13" s="10">
-        <v>9705.1355000000003</v>
+        <v>1970.3828000000001</v>
+      </c>
+      <c r="G13" s="11">
+        <v>3184.4783000000002</v>
+      </c>
+      <c r="H13" s="11">
+        <v>312.35219999999998</v>
+      </c>
+      <c r="I13" s="12">
+        <v>1585.7568000000001</v>
       </c>
       <c r="J13" s="11">
-        <v>8190.4983000000002</v>
-      </c>
-      <c r="K13" s="12">
-        <v>864.52800000000002</v>
-      </c>
-      <c r="L13" s="12">
-        <v>1226.4412</v>
-      </c>
-      <c r="M13" s="10">
-        <v>114.1075</v>
-      </c>
-      <c r="N13" s="10">
-        <v>106.6895</v>
-      </c>
-      <c r="O13" s="11">
-        <v>324.37099999999998</v>
-      </c>
-      <c r="P13" s="10">
-        <v>1636.0942</v>
+        <v>8068.1158999999998</v>
+      </c>
+      <c r="K13" s="11">
+        <v>786.73670000000004</v>
+      </c>
+      <c r="L13" s="11">
+        <v>1063.0753999999999</v>
+      </c>
+      <c r="M13" s="12">
+        <v>110.1891</v>
+      </c>
+      <c r="N13" s="12">
+        <v>2560.8975999999998</v>
+      </c>
+      <c r="O13" s="12">
+        <v>103.1523</v>
+      </c>
+      <c r="P13" s="12">
+        <v>9684.1633000000002</v>
       </c>
     </row>
     <row r="14" ht="14.25">
       <c r="A14" s="5">
-        <v>44143</v>
+        <v>44109</v>
       </c>
       <c r="B14" s="6">
-        <v>1300.3742</v>
+        <v>1270.1541</v>
       </c>
       <c r="C14" s="7">
-        <v>1785.0999999999999</v>
-      </c>
-      <c r="D14" s="6">
-        <v>1109.2917</v>
-      </c>
-      <c r="E14" s="6">
-        <v>1463.0225</v>
+        <v>1765.1811</v>
+      </c>
+      <c r="D14" s="8">
+        <v>1024.0264</v>
+      </c>
+      <c r="E14" s="8">
+        <v>1304.5077000000001</v>
       </c>
       <c r="F14" s="7">
-        <v>2099.2732000000001</v>
-      </c>
-      <c r="G14" s="8">
-        <v>3156.7636000000002</v>
-      </c>
-      <c r="H14" s="6">
-        <v>2666.2732000000001</v>
-      </c>
-      <c r="I14" s="6">
-        <v>9792.0668999999998</v>
+        <v>1994.8734999999999</v>
+      </c>
+      <c r="G14" s="7">
+        <v>3131.1507999999999</v>
+      </c>
+      <c r="H14" s="7">
+        <v>312.46199999999999</v>
+      </c>
+      <c r="I14" s="8">
+        <v>1582.1251</v>
       </c>
       <c r="J14" s="7">
-        <v>8209.2849000000006</v>
-      </c>
-      <c r="K14" s="8">
-        <v>868.80190000000005</v>
-      </c>
-      <c r="L14" s="8">
-        <v>1331.6333999999999</v>
-      </c>
-      <c r="M14" s="6">
-        <v>114.70829999999999</v>
-      </c>
-      <c r="N14" s="6">
-        <v>107.06</v>
-      </c>
-      <c r="O14" s="7">
-        <v>325.9436</v>
-      </c>
-      <c r="P14" s="6">
-        <v>1648.5849000000001</v>
+        <v>7952.9319999999998</v>
+      </c>
+      <c r="K14" s="7">
+        <v>782.42510000000004</v>
+      </c>
+      <c r="L14" s="7">
+        <v>1055.9277999999999</v>
+      </c>
+      <c r="M14" s="8">
+        <v>109.9628</v>
+      </c>
+      <c r="N14" s="8">
+        <v>2550.0853000000002</v>
+      </c>
+      <c r="O14" s="8">
+        <v>103.0843</v>
+      </c>
+      <c r="P14" s="8">
+        <v>9602.8233</v>
       </c>
     </row>
     <row r="15" ht="14.25">
       <c r="A15" s="9">
-        <v>44144</v>
+        <v>44110</v>
       </c>
       <c r="B15" s="10">
-        <v>1288.8558</v>
+        <v>1269.6976999999999</v>
       </c>
       <c r="C15" s="11">
-        <v>1780.9971</v>
-      </c>
-      <c r="D15" s="10">
-        <v>1155.9314999999999</v>
-      </c>
-      <c r="E15" s="10">
-        <v>1447.79</v>
+        <v>1765.0338999999999</v>
+      </c>
+      <c r="D15" s="12">
+        <v>1026.1014</v>
+      </c>
+      <c r="E15" s="12">
+        <v>1371.3332</v>
       </c>
       <c r="F15" s="11">
-        <v>2084.0126</v>
-      </c>
-      <c r="G15" s="12">
-        <v>3183.4475000000002</v>
-      </c>
-      <c r="H15" s="10">
-        <v>2697.8941</v>
-      </c>
-      <c r="I15" s="10">
-        <v>9774.8724000000002</v>
+        <v>2001.9589000000001</v>
+      </c>
+      <c r="G15" s="11">
+        <v>3135.9189000000001</v>
+      </c>
+      <c r="H15" s="11">
+        <v>313.22379999999998</v>
+      </c>
+      <c r="I15" s="12">
+        <v>1586.2942</v>
       </c>
       <c r="J15" s="11">
-        <v>8275.1301999999996</v>
-      </c>
-      <c r="K15" s="12">
-        <v>869.71929999999998</v>
-      </c>
-      <c r="L15" s="12">
-        <v>1390.4322</v>
-      </c>
-      <c r="M15" s="10">
-        <v>114.5429</v>
-      </c>
-      <c r="N15" s="10">
-        <v>106.58839999999999</v>
-      </c>
-      <c r="O15" s="11">
-        <v>325.33819999999997</v>
-      </c>
-      <c r="P15" s="10">
-        <v>1652.8079</v>
+        <v>7895.9092000000001</v>
+      </c>
+      <c r="K15" s="11">
+        <v>788.45849999999996</v>
+      </c>
+      <c r="L15" s="11">
+        <v>1064.0790999999999</v>
+      </c>
+      <c r="M15" s="12">
+        <v>110.2938</v>
+      </c>
+      <c r="N15" s="12">
+        <v>2540.7968999999998</v>
+      </c>
+      <c r="O15" s="12">
+        <v>103.2334</v>
+      </c>
+      <c r="P15" s="12">
+        <v>9577.0298999999995</v>
       </c>
     </row>
     <row r="16" ht="14.25">
       <c r="A16" s="5">
-        <v>44145</v>
+        <v>44111</v>
       </c>
       <c r="B16" s="6">
-        <v>1295.9706000000001</v>
+        <v>1275.223</v>
       </c>
       <c r="C16" s="7">
-        <v>1868.4249</v>
-      </c>
-      <c r="D16" s="6">
-        <v>1204.5070000000001</v>
-      </c>
-      <c r="E16" s="6">
-        <v>1447.1139000000001</v>
+        <v>1817.7067999999999</v>
+      </c>
+      <c r="D16" s="8">
+        <v>1031.1512</v>
+      </c>
+      <c r="E16" s="8">
+        <v>1447.2597000000001</v>
       </c>
       <c r="F16" s="7">
-        <v>2092.0803000000001</v>
-      </c>
-      <c r="G16" s="8">
-        <v>3224.3472999999999</v>
-      </c>
-      <c r="H16" s="6">
-        <v>2702.7822000000001</v>
-      </c>
-      <c r="I16" s="6">
-        <v>10251.228999999999</v>
+        <v>2079.9409000000001</v>
+      </c>
+      <c r="G16" s="7">
+        <v>3134.8917999999999</v>
+      </c>
+      <c r="H16" s="7">
+        <v>316.39830000000001</v>
+      </c>
+      <c r="I16" s="8">
+        <v>1600.9762000000001</v>
       </c>
       <c r="J16" s="7">
-        <v>8435.5277999999998</v>
-      </c>
-      <c r="K16" s="8">
-        <v>873.54499999999996</v>
-      </c>
-      <c r="L16" s="8">
-        <v>1499.9200000000001</v>
-      </c>
-      <c r="M16" s="6">
-        <v>115.8267</v>
-      </c>
-      <c r="N16" s="6">
-        <v>107.3175</v>
-      </c>
-      <c r="O16" s="7">
-        <v>330.39569999999998</v>
-      </c>
-      <c r="P16" s="6">
-        <v>1678.7918</v>
+        <v>7971.9926999999998</v>
+      </c>
+      <c r="K16" s="7">
+        <v>811.60050000000001</v>
+      </c>
+      <c r="L16" s="7">
+        <v>1070.9744000000001</v>
+      </c>
+      <c r="M16" s="8">
+        <v>111.3593</v>
+      </c>
+      <c r="N16" s="8">
+        <v>2540.5933</v>
+      </c>
+      <c r="O16" s="8">
+        <v>104.2668</v>
+      </c>
+      <c r="P16" s="8">
+        <v>9594.6939000000002</v>
       </c>
     </row>
     <row r="17" ht="14.25">
       <c r="A17" s="9">
-        <v>44146</v>
+        <v>44112</v>
       </c>
       <c r="B17" s="10">
-        <v>1310.8456000000001</v>
+        <v>1266.5146999999999</v>
       </c>
       <c r="C17" s="11">
-        <v>1915.7782</v>
-      </c>
-      <c r="D17" s="10">
-        <v>1254.1836000000001</v>
-      </c>
-      <c r="E17" s="10">
-        <v>1451.5053</v>
+        <v>1786.6639</v>
+      </c>
+      <c r="D17" s="12">
+        <v>1025.2267999999999</v>
+      </c>
+      <c r="E17" s="12">
+        <v>1402.6913999999999</v>
       </c>
       <c r="F17" s="11">
-        <v>2095.0039999999999</v>
-      </c>
-      <c r="G17" s="12">
-        <v>3424.5544</v>
-      </c>
-      <c r="H17" s="10">
-        <v>2709.9212000000002</v>
-      </c>
-      <c r="I17" s="10">
-        <v>10258.261699999999</v>
+        <v>2059.9034999999999</v>
+      </c>
+      <c r="G17" s="11">
+        <v>3121.5387999999998</v>
+      </c>
+      <c r="H17" s="11">
+        <v>314.74930000000001</v>
+      </c>
+      <c r="I17" s="12">
+        <v>1589.6393</v>
       </c>
       <c r="J17" s="11">
-        <v>8774.8484000000008</v>
-      </c>
-      <c r="K17" s="12">
-        <v>870.68960000000004</v>
-      </c>
-      <c r="L17" s="12">
-        <v>1649.7547</v>
-      </c>
-      <c r="M17" s="10">
-        <v>117.36660000000001</v>
-      </c>
-      <c r="N17" s="10">
-        <v>108.6431</v>
-      </c>
-      <c r="O17" s="11">
-        <v>335.62279999999998</v>
-      </c>
-      <c r="P17" s="10">
-        <v>1707.6799000000001</v>
+        <v>7897.6872000000003</v>
+      </c>
+      <c r="K17" s="11">
+        <v>843.31880000000001</v>
+      </c>
+      <c r="L17" s="11">
+        <v>1068.6090999999999</v>
+      </c>
+      <c r="M17" s="12">
+        <v>110.5462</v>
+      </c>
+      <c r="N17" s="12">
+        <v>2541.4466000000002</v>
+      </c>
+      <c r="O17" s="12">
+        <v>103.7047</v>
+      </c>
+      <c r="P17" s="12">
+        <v>9570.5301999999992</v>
       </c>
     </row>
     <row r="18" ht="14.25">
       <c r="A18" s="5">
+        <v>44115</v>
+      </c>
+      <c r="B18" s="6">
+        <v>1256.0193999999999</v>
+      </c>
+      <c r="C18" s="7">
+        <v>1748.4384</v>
+      </c>
+      <c r="D18" s="8">
+        <v>1015.9383</v>
+      </c>
+      <c r="E18" s="8">
+        <v>1374.9395</v>
+      </c>
+      <c r="F18" s="7">
+        <v>2039.027</v>
+      </c>
+      <c r="G18" s="7">
+        <v>3073.056</v>
+      </c>
+      <c r="H18" s="7">
+        <v>311.73840000000001</v>
+      </c>
+      <c r="I18" s="8">
+        <v>1576.2713000000001</v>
+      </c>
+      <c r="J18" s="7">
+        <v>7811.3186999999998</v>
+      </c>
+      <c r="K18" s="7">
+        <v>860.82169999999996</v>
+      </c>
+      <c r="L18" s="7">
+        <v>1048.9176</v>
+      </c>
+      <c r="M18" s="8">
+        <v>109.66</v>
+      </c>
+      <c r="N18" s="8">
+        <v>2532.5119</v>
+      </c>
+      <c r="O18" s="8">
+        <v>102.7916</v>
+      </c>
+      <c r="P18" s="8">
+        <v>9559.8189999999995</v>
+      </c>
+    </row>
+    <row r="19" ht="14.25">
+      <c r="A19" s="9">
+        <v>44116</v>
+      </c>
+      <c r="B19" s="10">
+        <v>1258.4091000000001</v>
+      </c>
+      <c r="C19" s="11">
+        <v>1755.3747000000001</v>
+      </c>
+      <c r="D19" s="12">
+        <v>1014.1052</v>
+      </c>
+      <c r="E19" s="12">
+        <v>1367.8235</v>
+      </c>
+      <c r="F19" s="11">
+        <v>2118.1439</v>
+      </c>
+      <c r="G19" s="11">
+        <v>3057.5410000000002</v>
+      </c>
+      <c r="H19" s="11">
+        <v>313.10989999999998</v>
+      </c>
+      <c r="I19" s="12">
+        <v>1578.0118</v>
+      </c>
+      <c r="J19" s="11">
+        <v>7799.1135999999997</v>
+      </c>
+      <c r="K19" s="11">
+        <v>849.15809999999999</v>
+      </c>
+      <c r="L19" s="11">
+        <v>1051.0821000000001</v>
+      </c>
+      <c r="M19" s="12">
+        <v>109.8783</v>
+      </c>
+      <c r="N19" s="12">
+        <v>2536.4454000000001</v>
+      </c>
+      <c r="O19" s="12">
+        <v>103.3944</v>
+      </c>
+      <c r="P19" s="12">
+        <v>9531.4498999999996</v>
+      </c>
+    </row>
+    <row r="20" ht="14.25">
+      <c r="A20" s="5">
+        <v>44117</v>
+      </c>
+      <c r="B20" s="6">
+        <v>1250.7082</v>
+      </c>
+      <c r="C20" s="7">
+        <v>1745.3153</v>
+      </c>
+      <c r="D20" s="8">
+        <v>1012.5999</v>
+      </c>
+      <c r="E20" s="8">
+        <v>1339.9786999999999</v>
+      </c>
+      <c r="F20" s="7">
+        <v>2109.5853999999999</v>
+      </c>
+      <c r="G20" s="7">
+        <v>3068.3766000000001</v>
+      </c>
+      <c r="H20" s="7">
+        <v>311.4135</v>
+      </c>
+      <c r="I20" s="8">
+        <v>1568.5949000000001</v>
+      </c>
+      <c r="J20" s="7">
+        <v>7750.7070000000003</v>
+      </c>
+      <c r="K20" s="7">
+        <v>832.85519999999997</v>
+      </c>
+      <c r="L20" s="7">
+        <v>1052.5708999999999</v>
+      </c>
+      <c r="M20" s="8">
+        <v>109.1345</v>
+      </c>
+      <c r="N20" s="8">
+        <v>2522.8173999999999</v>
+      </c>
+      <c r="O20" s="8">
+        <v>102.6996</v>
+      </c>
+      <c r="P20" s="8">
+        <v>9492.5079999999998</v>
+      </c>
+    </row>
+    <row r="21" ht="14.25">
+      <c r="A21" s="9">
+        <v>44118</v>
+      </c>
+      <c r="B21" s="10">
+        <v>1247.1222</v>
+      </c>
+      <c r="C21" s="11">
+        <v>1747.6957</v>
+      </c>
+      <c r="D21" s="12">
+        <v>1006.6968000000001</v>
+      </c>
+      <c r="E21" s="12">
+        <v>1323.9781</v>
+      </c>
+      <c r="F21" s="11">
+        <v>2067.6750999999999</v>
+      </c>
+      <c r="G21" s="11">
+        <v>3046.0437000000002</v>
+      </c>
+      <c r="H21" s="11">
+        <v>309.75049999999999</v>
+      </c>
+      <c r="I21" s="12">
+        <v>1561.1708000000001</v>
+      </c>
+      <c r="J21" s="11">
+        <v>7728.6229999999996</v>
+      </c>
+      <c r="K21" s="11">
+        <v>821.95060000000001</v>
+      </c>
+      <c r="L21" s="11">
+        <v>1048.8435999999999</v>
+      </c>
+      <c r="M21" s="12">
+        <v>108.627</v>
+      </c>
+      <c r="N21" s="12">
+        <v>2517.4976000000001</v>
+      </c>
+      <c r="O21" s="12">
+        <v>102.20010000000001</v>
+      </c>
+      <c r="P21" s="12">
+        <v>9459.0018999999993</v>
+      </c>
+    </row>
+    <row r="22" ht="14.25">
+      <c r="A22" s="5">
+        <v>44119</v>
+      </c>
+      <c r="B22" s="6">
+        <v>1249.0262</v>
+      </c>
+      <c r="C22" s="7">
+        <v>1731.8429000000001</v>
+      </c>
+      <c r="D22" s="8">
+        <v>1013.2426</v>
+      </c>
+      <c r="E22" s="8">
+        <v>1331.0802000000001</v>
+      </c>
+      <c r="F22" s="7">
+        <v>2056.5752000000002</v>
+      </c>
+      <c r="G22" s="7">
+        <v>3016.4893999999999</v>
+      </c>
+      <c r="H22" s="7">
+        <v>310.08449999999999</v>
+      </c>
+      <c r="I22" s="8">
+        <v>1562.4648999999999</v>
+      </c>
+      <c r="J22" s="7">
+        <v>7704.1983</v>
+      </c>
+      <c r="K22" s="7">
+        <v>821.63459999999998</v>
+      </c>
+      <c r="L22" s="7">
+        <v>1052.0322000000001</v>
+      </c>
+      <c r="M22" s="8">
+        <v>108.7094</v>
+      </c>
+      <c r="N22" s="8">
+        <v>2515.8939</v>
+      </c>
+      <c r="O22" s="8">
+        <v>102.264</v>
+      </c>
+      <c r="P22" s="8">
+        <v>9442.2011999999995</v>
+      </c>
+    </row>
+    <row r="23" ht="14.25">
+      <c r="A23" s="5">
+        <v>44122</v>
+      </c>
+      <c r="B23" s="13">
+        <v>1243.0021999999999</v>
+      </c>
+      <c r="C23" s="14">
+        <v>1730.0260000000001</v>
+      </c>
+      <c r="D23" s="13">
+        <v>1011.7074</v>
+      </c>
+      <c r="E23" s="13">
+        <v>1326.0165999999999</v>
+      </c>
+      <c r="F23" s="14">
+        <v>2027.3876</v>
+      </c>
+      <c r="G23" s="7">
+        <v>3002.0704999999998</v>
+      </c>
+      <c r="H23" s="13">
+        <v>2504.6623</v>
+      </c>
+      <c r="I23" s="13">
+        <v>9423.2183000000005</v>
+      </c>
+      <c r="J23" s="14">
+        <v>7735.7745999999997</v>
+      </c>
+      <c r="K23" s="7">
+        <v>820.0385</v>
+      </c>
+      <c r="L23" s="7">
+        <v>1065.23</v>
+      </c>
+      <c r="M23" s="13">
+        <v>108.2895</v>
+      </c>
+      <c r="N23" s="13">
+        <v>101.7206</v>
+      </c>
+      <c r="O23" s="14">
+        <v>308.2792</v>
+      </c>
+      <c r="P23" s="13">
+        <v>1556.8027999999999</v>
+      </c>
+    </row>
+    <row r="24" ht="14.25">
+      <c r="A24" s="9">
+        <v>44123</v>
+      </c>
+      <c r="B24" s="15">
+        <v>1250.6735000000001</v>
+      </c>
+      <c r="C24" s="16">
+        <v>1744.1883</v>
+      </c>
+      <c r="D24" s="15">
+        <v>1019.3059</v>
+      </c>
+      <c r="E24" s="15">
+        <v>1369.8780999999999</v>
+      </c>
+      <c r="F24" s="16">
+        <v>2057.8168000000001</v>
+      </c>
+      <c r="G24" s="11">
+        <v>3009.2399999999998</v>
+      </c>
+      <c r="H24" s="15">
+        <v>2515.3027000000002</v>
+      </c>
+      <c r="I24" s="15">
+        <v>9473.8101000000006</v>
+      </c>
+      <c r="J24" s="16">
+        <v>7835.2954</v>
+      </c>
+      <c r="K24" s="11">
+        <v>836.29459999999995</v>
+      </c>
+      <c r="L24" s="11">
+        <v>1063.5404000000001</v>
+      </c>
+      <c r="M24" s="15">
+        <v>109.42100000000001</v>
+      </c>
+      <c r="N24" s="15">
+        <v>102.6147</v>
+      </c>
+      <c r="O24" s="16">
+        <v>310.89850000000001</v>
+      </c>
+      <c r="P24" s="15">
+        <v>1570.3838000000001</v>
+      </c>
+    </row>
+    <row r="25" ht="14.25">
+      <c r="A25" s="5">
+        <v>44124</v>
+      </c>
+      <c r="B25" s="13">
+        <v>1258.4109000000001</v>
+      </c>
+      <c r="C25" s="14">
+        <v>1763.454</v>
+      </c>
+      <c r="D25" s="13">
+        <v>1030.7067999999999</v>
+      </c>
+      <c r="E25" s="13">
+        <v>1399.8406</v>
+      </c>
+      <c r="F25" s="14">
+        <v>2080.0038</v>
+      </c>
+      <c r="G25" s="7">
+        <v>3034.6017000000002</v>
+      </c>
+      <c r="H25" s="13">
+        <v>2531.7451999999998</v>
+      </c>
+      <c r="I25" s="13">
+        <v>9551.9256999999998</v>
+      </c>
+      <c r="J25" s="14">
+        <v>7891.0528999999997</v>
+      </c>
+      <c r="K25" s="7">
+        <v>844.89269999999999</v>
+      </c>
+      <c r="L25" s="7">
+        <v>1066.4971</v>
+      </c>
+      <c r="M25" s="13">
+        <v>110.3143</v>
+      </c>
+      <c r="N25" s="13">
+        <v>103.432</v>
+      </c>
+      <c r="O25" s="14">
+        <v>313.55270000000002</v>
+      </c>
+      <c r="P25" s="13">
+        <v>1583.7799</v>
+      </c>
+    </row>
+    <row r="26" ht="14.25">
+      <c r="A26" s="9">
+        <v>44125</v>
+      </c>
+      <c r="B26" s="15">
+        <v>1279.9563000000001</v>
+      </c>
+      <c r="C26" s="16">
+        <v>1748.4223999999999</v>
+      </c>
+      <c r="D26" s="15">
+        <v>1033.752</v>
+      </c>
+      <c r="E26" s="15">
+        <v>1385.7536</v>
+      </c>
+      <c r="F26" s="16">
+        <v>2090.0391</v>
+      </c>
+      <c r="G26" s="11">
+        <v>3028.2721999999999</v>
+      </c>
+      <c r="H26" s="15">
+        <v>2535.1552000000001</v>
+      </c>
+      <c r="I26" s="15">
+        <v>9609.8682000000008</v>
+      </c>
+      <c r="J26" s="16">
+        <v>7955.3289999999997</v>
+      </c>
+      <c r="K26" s="11">
+        <v>844.29160000000002</v>
+      </c>
+      <c r="L26" s="11">
+        <v>1089.8939</v>
+      </c>
+      <c r="M26" s="15">
+        <v>111.48099999999999</v>
+      </c>
+      <c r="N26" s="15">
+        <v>104.7525</v>
+      </c>
+      <c r="O26" s="16">
+        <v>316.65140000000002</v>
+      </c>
+      <c r="P26" s="15">
+        <v>1597.7149999999999</v>
+      </c>
+    </row>
+    <row r="27" ht="14.25">
+      <c r="A27" s="5">
+        <v>44126</v>
+      </c>
+      <c r="B27" s="13">
+        <v>1292.0539000000001</v>
+      </c>
+      <c r="C27" s="14">
+        <v>1734.3866</v>
+      </c>
+      <c r="D27" s="13">
+        <v>1039.0261</v>
+      </c>
+      <c r="E27" s="13">
+        <v>1379.3216</v>
+      </c>
+      <c r="F27" s="14">
+        <v>2091.7447999999999</v>
+      </c>
+      <c r="G27" s="7">
+        <v>3057.7514000000001</v>
+      </c>
+      <c r="H27" s="13">
+        <v>2535.9612000000002</v>
+      </c>
+      <c r="I27" s="13">
+        <v>9599.7705000000005</v>
+      </c>
+      <c r="J27" s="14">
+        <v>7993.8486999999996</v>
+      </c>
+      <c r="K27" s="7">
+        <v>849.67520000000002</v>
+      </c>
+      <c r="L27" s="7">
+        <v>1099.2276999999999</v>
+      </c>
+      <c r="M27" s="13">
+        <v>112.0997</v>
+      </c>
+      <c r="N27" s="13">
+        <v>105.3152</v>
+      </c>
+      <c r="O27" s="14">
+        <v>318.56229999999999</v>
+      </c>
+      <c r="P27" s="13">
+        <v>1606.2552000000001</v>
+      </c>
+    </row>
+    <row r="28" ht="14.25">
+      <c r="A28" s="9">
+        <v>44132</v>
+      </c>
+      <c r="B28" s="15">
+        <v>1347.2005999999999</v>
+      </c>
+      <c r="C28" s="16">
+        <v>1767.2349999999999</v>
+      </c>
+      <c r="D28" s="15">
+        <v>1053.5986</v>
+      </c>
+      <c r="E28" s="15">
+        <v>1383.1831999999999</v>
+      </c>
+      <c r="F28" s="16">
+        <v>2152.7168000000001</v>
+      </c>
+      <c r="G28" s="11">
+        <v>3078.6302999999998</v>
+      </c>
+      <c r="H28" s="15">
+        <v>2561.152</v>
+      </c>
+      <c r="I28" s="15">
+        <v>9710.4493000000002</v>
+      </c>
+      <c r="J28" s="16">
+        <v>8040.9139999999998</v>
+      </c>
+      <c r="K28" s="11">
+        <v>863.05719999999997</v>
+      </c>
+      <c r="L28" s="11">
+        <v>1090.4014</v>
+      </c>
+      <c r="M28" s="15">
+        <v>115.3723</v>
+      </c>
+      <c r="N28" s="15">
+        <v>108.6108</v>
+      </c>
+      <c r="O28" s="16">
+        <v>327.76859999999999</v>
+      </c>
+      <c r="P28" s="15">
+        <v>1647.4595999999999</v>
+      </c>
+    </row>
+    <row r="29" ht="14.25">
+      <c r="A29" s="5">
+        <v>44133</v>
+      </c>
+      <c r="B29" s="13">
+        <v>1340.9271000000001</v>
+      </c>
+      <c r="C29" s="14">
+        <v>1751.8191999999999</v>
+      </c>
+      <c r="D29" s="13">
+        <v>1059.4296999999999</v>
+      </c>
+      <c r="E29" s="13">
+        <v>1389.9331</v>
+      </c>
+      <c r="F29" s="14">
+        <v>2135.8955999999998</v>
+      </c>
+      <c r="G29" s="7">
+        <v>3043.7838000000002</v>
+      </c>
+      <c r="H29" s="13">
+        <v>2573.8876</v>
+      </c>
+      <c r="I29" s="13">
+        <v>9719.3099999999995</v>
+      </c>
+      <c r="J29" s="14">
+        <v>8080.8068999999996</v>
+      </c>
+      <c r="K29" s="7">
+        <v>860.43230000000005</v>
+      </c>
+      <c r="L29" s="7">
+        <v>1105.3524</v>
+      </c>
+      <c r="M29" s="13">
+        <v>115.1695</v>
+      </c>
+      <c r="N29" s="13">
+        <v>108.5177</v>
+      </c>
+      <c r="O29" s="14">
+        <v>328.04239999999999</v>
+      </c>
+      <c r="P29" s="13">
+        <v>1645.6790000000001</v>
+      </c>
+    </row>
+    <row r="30" ht="14.25">
+      <c r="A30" s="9">
+        <v>44136</v>
+      </c>
+      <c r="B30" s="15">
+        <v>1326.3777</v>
+      </c>
+      <c r="C30" s="16">
+        <v>1736.53</v>
+      </c>
+      <c r="D30" s="15">
+        <v>1064.7896000000001</v>
+      </c>
+      <c r="E30" s="15">
+        <v>1409.2402999999999</v>
+      </c>
+      <c r="F30" s="16">
+        <v>2128.9187999999999</v>
+      </c>
+      <c r="G30" s="11">
+        <v>3028.5708</v>
+      </c>
+      <c r="H30" s="15">
+        <v>2603.2926000000002</v>
+      </c>
+      <c r="I30" s="15">
+        <v>9711.8593000000001</v>
+      </c>
+      <c r="J30" s="16">
+        <v>8091.2551000000003</v>
+      </c>
+      <c r="K30" s="11">
+        <v>858.25580000000002</v>
+      </c>
+      <c r="L30" s="11">
+        <v>1129.7229</v>
+      </c>
+      <c r="M30" s="15">
+        <v>114.7953</v>
+      </c>
+      <c r="N30" s="15">
+        <v>107.907</v>
+      </c>
+      <c r="O30" s="16">
+        <v>326.63279999999997</v>
+      </c>
+      <c r="P30" s="15">
+        <v>1640.9593</v>
+      </c>
+    </row>
+    <row r="31" ht="14.25">
+      <c r="A31" s="5">
+        <v>44137</v>
+      </c>
+      <c r="B31" s="13">
+        <v>1314.7537</v>
+      </c>
+      <c r="C31" s="14">
+        <v>1745.8626999999999</v>
+      </c>
+      <c r="D31" s="13">
+        <v>1061.5012999999999</v>
+      </c>
+      <c r="E31" s="13">
+        <v>1409.7791999999999</v>
+      </c>
+      <c r="F31" s="14">
+        <v>2128.6161999999999</v>
+      </c>
+      <c r="G31" s="7">
+        <v>3032.4544000000001</v>
+      </c>
+      <c r="H31" s="13">
+        <v>2665.5909000000001</v>
+      </c>
+      <c r="I31" s="13">
+        <v>9702.4599999999991</v>
+      </c>
+      <c r="J31" s="14">
+        <v>8118.5070999999998</v>
+      </c>
+      <c r="K31" s="7">
+        <v>862.21140000000003</v>
+      </c>
+      <c r="L31" s="7">
+        <v>1164.24</v>
+      </c>
+      <c r="M31" s="13">
+        <v>114.4892</v>
+      </c>
+      <c r="N31" s="13">
+        <v>107.5675</v>
+      </c>
+      <c r="O31" s="14">
+        <v>325.46409999999997</v>
+      </c>
+      <c r="P31" s="13">
+        <v>1637.6311000000001</v>
+      </c>
+    </row>
+    <row r="32" ht="14.25">
+      <c r="A32" s="9">
+        <v>44138</v>
+      </c>
+      <c r="B32" s="15">
+        <v>1312.5835999999999</v>
+      </c>
+      <c r="C32" s="16">
+        <v>1747.8268</v>
+      </c>
+      <c r="D32" s="15">
+        <v>1076.3024</v>
+      </c>
+      <c r="E32" s="15">
+        <v>1416.921</v>
+      </c>
+      <c r="F32" s="16">
+        <v>2112.4022</v>
+      </c>
+      <c r="G32" s="11">
+        <v>3038.4056999999998</v>
+      </c>
+      <c r="H32" s="15">
+        <v>2672.4218000000001</v>
+      </c>
+      <c r="I32" s="15">
+        <v>9716.4567999999999</v>
+      </c>
+      <c r="J32" s="16">
+        <v>8295.3667999999998</v>
+      </c>
+      <c r="K32" s="11">
+        <v>867.60789999999997</v>
+      </c>
+      <c r="L32" s="11">
+        <v>1220.1588999999999</v>
+      </c>
+      <c r="M32" s="15">
+        <v>114.5771</v>
+      </c>
+      <c r="N32" s="15">
+        <v>107.5385</v>
+      </c>
+      <c r="O32" s="16">
+        <v>326.6044</v>
+      </c>
+      <c r="P32" s="15">
+        <v>1643.0351000000001</v>
+      </c>
+    </row>
+    <row r="33" ht="14.25">
+      <c r="A33" s="5">
+        <v>44139</v>
+      </c>
+      <c r="B33" s="13">
+        <v>1309.5478000000001</v>
+      </c>
+      <c r="C33" s="14">
+        <v>1752.4931999999999</v>
+      </c>
+      <c r="D33" s="13">
+        <v>1081.6943000000001</v>
+      </c>
+      <c r="E33" s="13">
+        <v>1418.5012999999999</v>
+      </c>
+      <c r="F33" s="14">
+        <v>2100.9791</v>
+      </c>
+      <c r="G33" s="7">
+        <v>3038.2975000000001</v>
+      </c>
+      <c r="H33" s="13">
+        <v>2668.759</v>
+      </c>
+      <c r="I33" s="13">
+        <v>9703.7829999999994</v>
+      </c>
+      <c r="J33" s="14">
+        <v>8206.6826000000001</v>
+      </c>
+      <c r="K33" s="7">
+        <v>864.72490000000005</v>
+      </c>
+      <c r="L33" s="7">
+        <v>1245.4697000000001</v>
+      </c>
+      <c r="M33" s="13">
+        <v>114.35899999999999</v>
+      </c>
+      <c r="N33" s="13">
+        <v>107.34820000000001</v>
+      </c>
+      <c r="O33" s="14">
+        <v>326.49790000000002</v>
+      </c>
+      <c r="P33" s="13">
+        <v>1640.6425999999999</v>
+      </c>
+    </row>
+    <row r="34" ht="14.25">
+      <c r="A34" s="9">
+        <v>44140</v>
+      </c>
+      <c r="B34" s="15">
+        <v>1301.5358000000001</v>
+      </c>
+      <c r="C34" s="16">
+        <v>1757.3549</v>
+      </c>
+      <c r="D34" s="15">
+        <v>1080.8372999999999</v>
+      </c>
+      <c r="E34" s="15">
+        <v>1432.4299000000001</v>
+      </c>
+      <c r="F34" s="16">
+        <v>2106.0338000000002</v>
+      </c>
+      <c r="G34" s="11">
+        <v>3034.0862999999999</v>
+      </c>
+      <c r="H34" s="15">
+        <v>2655.4198999999999</v>
+      </c>
+      <c r="I34" s="15">
+        <v>9705.1355000000003</v>
+      </c>
+      <c r="J34" s="16">
+        <v>8190.4983000000002</v>
+      </c>
+      <c r="K34" s="11">
+        <v>864.52800000000002</v>
+      </c>
+      <c r="L34" s="11">
+        <v>1226.4412</v>
+      </c>
+      <c r="M34" s="15">
+        <v>114.1075</v>
+      </c>
+      <c r="N34" s="15">
+        <v>106.6895</v>
+      </c>
+      <c r="O34" s="16">
+        <v>324.37099999999998</v>
+      </c>
+      <c r="P34" s="15">
+        <v>1636.0942</v>
+      </c>
+    </row>
+    <row r="35" ht="14.25">
+      <c r="A35" s="5">
+        <v>44143</v>
+      </c>
+      <c r="B35" s="13">
+        <v>1300.3742</v>
+      </c>
+      <c r="C35" s="14">
+        <v>1785.0999999999999</v>
+      </c>
+      <c r="D35" s="13">
+        <v>1109.2917</v>
+      </c>
+      <c r="E35" s="13">
+        <v>1463.0225</v>
+      </c>
+      <c r="F35" s="14">
+        <v>2099.2732000000001</v>
+      </c>
+      <c r="G35" s="7">
+        <v>3156.7636000000002</v>
+      </c>
+      <c r="H35" s="13">
+        <v>2666.2732000000001</v>
+      </c>
+      <c r="I35" s="13">
+        <v>9792.0668999999998</v>
+      </c>
+      <c r="J35" s="14">
+        <v>8209.2849000000006</v>
+      </c>
+      <c r="K35" s="7">
+        <v>868.80190000000005</v>
+      </c>
+      <c r="L35" s="7">
+        <v>1331.6333999999999</v>
+      </c>
+      <c r="M35" s="13">
+        <v>114.70829999999999</v>
+      </c>
+      <c r="N35" s="13">
+        <v>107.06</v>
+      </c>
+      <c r="O35" s="14">
+        <v>325.9436</v>
+      </c>
+      <c r="P35" s="13">
+        <v>1648.5849000000001</v>
+      </c>
+    </row>
+    <row r="36" ht="14.25">
+      <c r="A36" s="9">
+        <v>44144</v>
+      </c>
+      <c r="B36" s="15">
+        <v>1288.8558</v>
+      </c>
+      <c r="C36" s="16">
+        <v>1780.9971</v>
+      </c>
+      <c r="D36" s="15">
+        <v>1155.9314999999999</v>
+      </c>
+      <c r="E36" s="15">
+        <v>1447.79</v>
+      </c>
+      <c r="F36" s="16">
+        <v>2084.0126</v>
+      </c>
+      <c r="G36" s="11">
+        <v>3183.4475000000002</v>
+      </c>
+      <c r="H36" s="15">
+        <v>2697.8941</v>
+      </c>
+      <c r="I36" s="15">
+        <v>9774.8724000000002</v>
+      </c>
+      <c r="J36" s="16">
+        <v>8275.1301999999996</v>
+      </c>
+      <c r="K36" s="11">
+        <v>869.71929999999998</v>
+      </c>
+      <c r="L36" s="11">
+        <v>1390.4322</v>
+      </c>
+      <c r="M36" s="15">
+        <v>114.5429</v>
+      </c>
+      <c r="N36" s="15">
+        <v>106.58839999999999</v>
+      </c>
+      <c r="O36" s="16">
+        <v>325.33819999999997</v>
+      </c>
+      <c r="P36" s="15">
+        <v>1652.8079</v>
+      </c>
+    </row>
+    <row r="37" ht="14.25">
+      <c r="A37" s="5">
+        <v>44145</v>
+      </c>
+      <c r="B37" s="13">
+        <v>1295.9706000000001</v>
+      </c>
+      <c r="C37" s="14">
+        <v>1868.4249</v>
+      </c>
+      <c r="D37" s="13">
+        <v>1204.5070000000001</v>
+      </c>
+      <c r="E37" s="13">
+        <v>1447.1139000000001</v>
+      </c>
+      <c r="F37" s="14">
+        <v>2092.0803000000001</v>
+      </c>
+      <c r="G37" s="7">
+        <v>3224.3472999999999</v>
+      </c>
+      <c r="H37" s="13">
+        <v>2702.7822000000001</v>
+      </c>
+      <c r="I37" s="13">
+        <v>10251.228999999999</v>
+      </c>
+      <c r="J37" s="14">
+        <v>8435.5277999999998</v>
+      </c>
+      <c r="K37" s="7">
+        <v>873.54499999999996</v>
+      </c>
+      <c r="L37" s="7">
+        <v>1499.9200000000001</v>
+      </c>
+      <c r="M37" s="13">
+        <v>115.8267</v>
+      </c>
+      <c r="N37" s="13">
+        <v>107.3175</v>
+      </c>
+      <c r="O37" s="14">
+        <v>330.39569999999998</v>
+      </c>
+      <c r="P37" s="13">
+        <v>1678.7918</v>
+      </c>
+    </row>
+    <row r="38" ht="14.25">
+      <c r="A38" s="9">
+        <v>44146</v>
+      </c>
+      <c r="B38" s="15">
+        <v>1310.8456000000001</v>
+      </c>
+      <c r="C38" s="16">
+        <v>1915.7782</v>
+      </c>
+      <c r="D38" s="15">
+        <v>1254.1836000000001</v>
+      </c>
+      <c r="E38" s="15">
+        <v>1451.5053</v>
+      </c>
+      <c r="F38" s="16">
+        <v>2095.0039999999999</v>
+      </c>
+      <c r="G38" s="11">
+        <v>3424.5544</v>
+      </c>
+      <c r="H38" s="15">
+        <v>2709.9212000000002</v>
+      </c>
+      <c r="I38" s="15">
+        <v>10258.261699999999</v>
+      </c>
+      <c r="J38" s="16">
+        <v>8774.8484000000008</v>
+      </c>
+      <c r="K38" s="11">
+        <v>870.68960000000004</v>
+      </c>
+      <c r="L38" s="11">
+        <v>1649.7547</v>
+      </c>
+      <c r="M38" s="15">
+        <v>117.36660000000001</v>
+      </c>
+      <c r="N38" s="15">
+        <v>108.6431</v>
+      </c>
+      <c r="O38" s="16">
+        <v>335.62279999999998</v>
+      </c>
+      <c r="P38" s="15">
+        <v>1707.6799000000001</v>
+      </c>
+    </row>
+    <row r="39" ht="14.25">
+      <c r="A39" s="5">
         <v>44147</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B39" s="13">
         <v>1321.0592999999999</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C39" s="14">
         <v>1897.3658</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D39" s="13">
         <v>1282.5717</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E39" s="13">
         <v>1444.9938</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F39" s="14">
         <v>2090.5378000000001</v>
       </c>
-      <c r="G18" s="8">
+      <c r="G39" s="7">
         <v>3393.6965</v>
       </c>
-      <c r="H18" s="6">
+      <c r="H39" s="13">
         <v>2708.2085999999999</v>
       </c>
-      <c r="I18" s="6">
+      <c r="I39" s="13">
         <v>10230.309600000001</v>
       </c>
-      <c r="J18" s="7">
+      <c r="J39" s="14">
         <v>8814.0038000000004</v>
       </c>
-      <c r="K18" s="8">
+      <c r="K39" s="7">
         <v>867.03920000000005</v>
       </c>
-      <c r="L18" s="8">
+      <c r="L39" s="7">
         <v>1814.4662000000001</v>
       </c>
-      <c r="M18" s="6">
+      <c r="M39" s="13">
         <v>117.8215</v>
       </c>
-      <c r="N18" s="6">
+      <c r="N39" s="13">
         <v>109.2805</v>
       </c>
-      <c r="O18" s="7">
+      <c r="O39" s="14">
         <v>339.0926</v>
       </c>
-      <c r="P18" s="6">
+      <c r="P39" s="13">
         <v>1718.4973</v>
       </c>
     </row>
@@ -1709,40 +2765,40 @@
       <c r="A2" s="5">
         <v>44122</v>
       </c>
-      <c r="B2" s="13">
+      <c r="B2" s="8">
         <v>951775.46999999997</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="7">
         <v>72823.029999999999</v>
       </c>
-      <c r="D2" s="13">
+      <c r="D2" s="8">
         <v>22873.48</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="7">
         <v>271780.34999999998</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="7">
         <v>137821.72</v>
       </c>
-      <c r="G2" s="13">
+      <c r="G2" s="8">
         <v>6196.3800000000001</v>
       </c>
-      <c r="H2" s="8">
+      <c r="H2" s="7">
         <v>144873.16</v>
       </c>
-      <c r="I2" s="8">
+      <c r="I2" s="7">
         <v>74625</v>
       </c>
-      <c r="J2" s="13">
+      <c r="J2" s="8">
         <v>27362.07</v>
       </c>
-      <c r="K2" s="13">
+      <c r="K2" s="8">
         <v>175405.20000000001</v>
       </c>
-      <c r="L2" s="13">
+      <c r="L2" s="8">
         <v>193165.54000000001</v>
       </c>
-      <c r="M2" s="14">
+      <c r="M2" s="17">
         <v>2078701.3999999999</v>
       </c>
     </row>
@@ -1750,40 +2806,40 @@
       <c r="A3" s="9">
         <v>44123</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B3" s="12">
         <v>957649.45999999996</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="11">
         <v>72996.949999999997</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="12">
         <v>23060.73</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="11">
         <v>273821.56</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="11">
         <v>142380.54000000001</v>
       </c>
-      <c r="G3" s="15">
+      <c r="G3" s="12">
         <v>6186.5500000000002</v>
       </c>
-      <c r="H3" s="12">
+      <c r="H3" s="11">
         <v>146736.95000000001</v>
       </c>
-      <c r="I3" s="12">
+      <c r="I3" s="11">
         <v>75745.050000000003</v>
       </c>
-      <c r="J3" s="15">
+      <c r="J3" s="12">
         <v>27904.490000000002</v>
       </c>
-      <c r="K3" s="15">
+      <c r="K3" s="12">
         <v>176150.35999999999</v>
       </c>
-      <c r="L3" s="15">
+      <c r="L3" s="12">
         <v>194202.62</v>
       </c>
-      <c r="M3" s="16">
+      <c r="M3" s="18">
         <v>2096835.2600000002</v>
       </c>
     </row>
@@ -1791,40 +2847,40 @@
       <c r="A4" s="5">
         <v>44124</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4" s="8">
         <v>963574</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="7">
         <v>73612.160000000003</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="8">
         <v>23315.450000000001</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="7">
         <v>276884.27000000002</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="7">
         <v>145494.73999999999</v>
       </c>
-      <c r="G4" s="13">
+      <c r="G4" s="8">
         <v>6203.75</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="7">
         <v>147781.16</v>
       </c>
-      <c r="I4" s="8">
+      <c r="I4" s="7">
         <v>76561.720000000001</v>
       </c>
-      <c r="J4" s="13">
+      <c r="J4" s="8">
         <v>28191.369999999999</v>
       </c>
-      <c r="K4" s="13">
+      <c r="K4" s="8">
         <v>178393.95000000001</v>
       </c>
-      <c r="L4" s="13">
+      <c r="L4" s="8">
         <v>195803.89999999999</v>
       </c>
-      <c r="M4" s="14">
+      <c r="M4" s="17">
         <v>2115816.4700000002</v>
       </c>
     </row>
@@ -1832,40 +2888,40 @@
       <c r="A5" s="9">
         <v>44125</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B5" s="12">
         <v>980071.48999999999</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="11">
         <v>73458.619999999995</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="12">
         <v>23116.709999999999</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="11">
         <v>277702.29999999999</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="11">
         <v>144030.57999999999</v>
       </c>
-      <c r="G5" s="15">
+      <c r="G5" s="12">
         <v>6339.8500000000004</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="11">
         <v>148984.89999999999</v>
       </c>
-      <c r="I5" s="12">
+      <c r="I5" s="11">
         <v>76931.110000000001</v>
       </c>
-      <c r="J5" s="15">
+      <c r="J5" s="12">
         <v>28171.32</v>
       </c>
-      <c r="K5" s="15">
+      <c r="K5" s="12">
         <v>178634.22</v>
       </c>
-      <c r="L5" s="15">
+      <c r="L5" s="12">
         <v>196991.66</v>
       </c>
-      <c r="M5" s="16">
+      <c r="M5" s="18">
         <v>2134432.7600000002</v>
       </c>
     </row>
@@ -1873,40 +2929,40 @@
       <c r="A6" s="5">
         <v>44126</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6" s="8">
         <v>989334.69999999995</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="7">
         <v>74173.720000000001</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="8">
         <v>22931.130000000001</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="7">
         <v>279119.12</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="7">
         <v>143362.06</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="8">
         <v>6394.1400000000003</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="7">
         <v>149706.29000000001</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I6" s="7">
         <v>76993.889999999999</v>
       </c>
-      <c r="J6" s="13">
+      <c r="J6" s="8">
         <v>28521.970000000001</v>
       </c>
-      <c r="K6" s="13">
+      <c r="K6" s="8">
         <v>178691.01999999999</v>
       </c>
-      <c r="L6" s="13">
+      <c r="L6" s="8">
         <v>196784.67000000001</v>
       </c>
-      <c r="M6" s="14">
+      <c r="M6" s="17">
         <v>2146012.71</v>
       </c>
     </row>
@@ -1914,40 +2970,40 @@
       <c r="A7" s="9">
         <v>44132</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="12">
         <v>1031560.9399999999</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="11">
         <v>74680.190000000002</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="12">
         <v>23365.439999999999</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="11">
         <v>283033.79999999999</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="11">
         <v>143763.42000000001</v>
       </c>
-      <c r="G7" s="15">
+      <c r="G7" s="12">
         <v>6342.8000000000002</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="11">
         <v>150587.70999999999</v>
       </c>
-      <c r="I7" s="12">
+      <c r="I7" s="11">
         <v>79238.179999999993</v>
       </c>
-      <c r="J7" s="15">
+      <c r="J7" s="12">
         <v>28971.189999999999</v>
       </c>
-      <c r="K7" s="15">
+      <c r="K7" s="12">
         <v>180466.03</v>
       </c>
-      <c r="L7" s="15">
+      <c r="L7" s="12">
         <v>199053.45999999999</v>
       </c>
-      <c r="M7" s="16">
+      <c r="M7" s="18">
         <v>2201063.1599999997</v>
       </c>
     </row>
@@ -1955,40 +3011,40 @@
       <c r="A8" s="5">
         <v>44133</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8" s="8">
         <v>1026757.26</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="7">
         <v>73834.899999999994</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="8">
         <v>23161.619999999999</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="7">
         <v>284600.25</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="7">
         <v>146413.84</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G8" s="8">
         <v>6429.7700000000004</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="7">
         <v>151334.75</v>
       </c>
-      <c r="I8" s="8">
+      <c r="I8" s="7">
         <v>78619.020000000004</v>
       </c>
-      <c r="J8" s="13">
+      <c r="J8" s="8">
         <v>28883.07</v>
       </c>
-      <c r="K8" s="13">
+      <c r="K8" s="8">
         <v>182485.82999999999</v>
       </c>
-      <c r="L8" s="13">
+      <c r="L8" s="8">
         <v>199235.10000000001</v>
       </c>
-      <c r="M8" s="14">
+      <c r="M8" s="17">
         <v>2201755.4100000001</v>
       </c>
     </row>
@@ -1996,40 +3052,40 @@
       <c r="A9" s="9">
         <v>44136</v>
       </c>
-      <c r="B9" s="15">
+      <c r="B9" s="12">
         <v>1015616.7</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="11">
         <v>73465.869999999995</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="12">
         <v>22959.470000000001</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="11">
         <v>286040.10999999999</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9" s="11">
         <v>148447.63</v>
       </c>
-      <c r="G9" s="15">
+      <c r="G9" s="12">
         <v>6571.5299999999997</v>
       </c>
-      <c r="H9" s="12">
+      <c r="H9" s="11">
         <v>151530.42000000001</v>
       </c>
-      <c r="I9" s="12">
+      <c r="I9" s="11">
         <v>78362.210000000006</v>
       </c>
-      <c r="J9" s="15">
+      <c r="J9" s="12">
         <v>28810.009999999998</v>
       </c>
-      <c r="K9" s="15">
+      <c r="K9" s="12">
         <v>184557.79000000001</v>
       </c>
-      <c r="L9" s="15">
+      <c r="L9" s="12">
         <v>199082.37</v>
       </c>
-      <c r="M9" s="16">
+      <c r="M9" s="18">
         <v>2195444.1099999999</v>
       </c>
     </row>
@@ -2037,40 +3093,40 @@
       <c r="A10" s="5">
         <v>44137</v>
       </c>
-      <c r="B10" s="13">
+      <c r="B10" s="8">
         <v>1006716.15</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="7">
         <v>73560.070000000007</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="8">
         <v>23082.869999999999</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="7">
         <v>285156.75</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="7">
         <v>148504.39999999999</v>
       </c>
-      <c r="G10" s="13">
+      <c r="G10" s="8">
         <v>6772.3199999999997</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H10" s="7">
         <v>152040.79000000001</v>
       </c>
-      <c r="I10" s="8">
+      <c r="I10" s="7">
         <v>78351.070000000007</v>
       </c>
-      <c r="J10" s="13">
+      <c r="J10" s="8">
         <v>28942.790000000001</v>
       </c>
-      <c r="K10" s="13">
+      <c r="K10" s="8">
         <v>188974.37</v>
       </c>
-      <c r="L10" s="13">
+      <c r="L10" s="8">
         <v>198889.69</v>
       </c>
-      <c r="M10" s="14">
+      <c r="M10" s="17">
         <v>2190991.27</v>
       </c>
     </row>
@@ -2078,40 +3134,40 @@
       <c r="A11" s="9">
         <v>44138</v>
       </c>
-      <c r="B11" s="15">
+      <c r="B11" s="12">
         <v>1005054.49</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="11">
         <v>73704.440000000002</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="12">
         <v>23108.830000000002</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="11">
         <v>289132.84000000003</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11" s="11">
         <v>149256.70999999999</v>
       </c>
-      <c r="G11" s="15">
+      <c r="G11" s="12">
         <v>7097.5900000000001</v>
       </c>
-      <c r="H11" s="12">
+      <c r="H11" s="11">
         <v>155352.95999999999</v>
       </c>
-      <c r="I11" s="12">
+      <c r="I11" s="11">
         <v>77754.259999999995</v>
       </c>
-      <c r="J11" s="15">
+      <c r="J11" s="12">
         <v>29123.939999999999</v>
       </c>
-      <c r="K11" s="15">
+      <c r="K11" s="12">
         <v>189458.64000000001</v>
       </c>
-      <c r="L11" s="15">
+      <c r="L11" s="12">
         <v>199176.60999999999</v>
       </c>
-      <c r="M11" s="16">
+      <c r="M11" s="18">
         <v>2198221.3100000001</v>
       </c>
     </row>
@@ -2119,40 +3175,40 @@
       <c r="A12" s="5">
         <v>44139</v>
       </c>
-      <c r="B12" s="13">
+      <c r="B12" s="8">
         <v>1002729.92</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="7">
         <v>73701.809999999998</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="8">
         <v>23170.529999999999</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="7">
         <v>290581.31</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="7">
         <v>149423.17999999999</v>
       </c>
-      <c r="G12" s="13">
+      <c r="G12" s="8">
         <v>7244.8299999999999</v>
       </c>
-      <c r="H12" s="8">
+      <c r="H12" s="7">
         <v>153692.10999999999</v>
       </c>
-      <c r="I12" s="8">
+      <c r="I12" s="7">
         <v>77333.789999999994</v>
       </c>
-      <c r="J12" s="13">
+      <c r="J12" s="8">
         <v>29027.169999999998</v>
       </c>
-      <c r="K12" s="13">
+      <c r="K12" s="8">
         <v>189198.97</v>
       </c>
-      <c r="L12" s="13">
+      <c r="L12" s="8">
         <v>198916.81</v>
       </c>
-      <c r="M12" s="14">
+      <c r="M12" s="17">
         <v>2195020.4299999997</v>
       </c>
     </row>
@@ -2160,40 +3216,40 @@
       <c r="A13" s="9">
         <v>44140</v>
       </c>
-      <c r="B13" s="15">
+      <c r="B13" s="12">
         <v>996595.06000000006</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C13" s="11">
         <v>73599.660000000003</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="12">
         <v>23234.810000000001</v>
       </c>
-      <c r="E13" s="12">
+      <c r="E13" s="11">
         <v>290351.08000000002</v>
       </c>
-      <c r="F13" s="12">
+      <c r="F13" s="11">
         <v>150890.39999999999</v>
       </c>
-      <c r="G13" s="15">
+      <c r="G13" s="12">
         <v>7134.1400000000003</v>
       </c>
-      <c r="H13" s="12">
+      <c r="H13" s="11">
         <v>156802.26999999999</v>
       </c>
-      <c r="I13" s="12">
+      <c r="I13" s="11">
         <v>77519.850000000006</v>
       </c>
-      <c r="J13" s="15">
+      <c r="J13" s="12">
         <v>29020.560000000001</v>
       </c>
-      <c r="K13" s="15">
+      <c r="K13" s="12">
         <v>188253.31</v>
       </c>
-      <c r="L13" s="15">
+      <c r="L13" s="12">
         <v>198944.5</v>
       </c>
-      <c r="M13" s="16">
+      <c r="M13" s="18">
         <v>2192345.6400000001</v>
       </c>
     </row>
@@ -2201,40 +3257,40 @@
       <c r="A14" s="5">
         <v>44143</v>
       </c>
-      <c r="B14" s="13">
+      <c r="B14" s="8">
         <v>995705.66000000003</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="7">
         <v>76575.520000000004</v>
       </c>
-      <c r="D14" s="13">
+      <c r="D14" s="8">
         <v>23601.639999999999</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14" s="7">
         <v>297994.92999999999</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F14" s="7">
         <v>154112.98999999999</v>
       </c>
-      <c r="G14" s="13">
+      <c r="G14" s="8">
         <v>7746.04</v>
       </c>
-      <c r="H14" s="8">
+      <c r="H14" s="7">
         <v>157161.92000000001</v>
       </c>
-      <c r="I14" s="8">
+      <c r="I14" s="7">
         <v>77271</v>
       </c>
-      <c r="J14" s="13">
+      <c r="J14" s="8">
         <v>29164.02</v>
       </c>
-      <c r="K14" s="13">
+      <c r="K14" s="8">
         <v>189022.73999999999</v>
       </c>
-      <c r="L14" s="13">
+      <c r="L14" s="8">
         <v>200726.48999999999</v>
       </c>
-      <c r="M14" s="14">
+      <c r="M14" s="17">
         <v>2209082.9499999997</v>
       </c>
     </row>
@@ -2242,40 +3298,40 @@
       <c r="A15" s="9">
         <v>44144</v>
       </c>
-      <c r="B15" s="15">
+      <c r="B15" s="12">
         <v>986885.88</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15" s="11">
         <v>77222.800000000003</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15" s="12">
         <v>23547.389999999999</v>
       </c>
-      <c r="E15" s="12">
+      <c r="E15" s="11">
         <v>310524.03999999998</v>
       </c>
-      <c r="F15" s="12">
+      <c r="F15" s="11">
         <v>152508.41</v>
       </c>
-      <c r="G15" s="15">
+      <c r="G15" s="12">
         <v>8088.0699999999997</v>
       </c>
-      <c r="H15" s="12">
+      <c r="H15" s="11">
         <v>158422.48999999999</v>
       </c>
-      <c r="I15" s="12">
+      <c r="I15" s="11">
         <v>76709.279999999999</v>
       </c>
-      <c r="J15" s="15">
+      <c r="J15" s="12">
         <v>29194.82</v>
       </c>
-      <c r="K15" s="15">
+      <c r="K15" s="12">
         <v>191264.47</v>
       </c>
-      <c r="L15" s="15">
+      <c r="L15" s="12">
         <v>200374.03</v>
       </c>
-      <c r="M15" s="16">
+      <c r="M15" s="18">
         <v>2214741.6799999997</v>
       </c>
     </row>
@@ -2283,40 +3339,40 @@
       <c r="A16" s="5">
         <v>44145</v>
       </c>
-      <c r="B16" s="13">
+      <c r="B16" s="8">
         <v>992333.80000000005</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="7">
         <v>78214.929999999993</v>
       </c>
-      <c r="D16" s="13">
+      <c r="D16" s="8">
         <v>24703.32</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E16" s="7">
         <v>323573.12</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F16" s="7">
         <v>152437.19</v>
       </c>
-      <c r="G16" s="13">
+      <c r="G16" s="8">
         <v>8724.9500000000007</v>
       </c>
-      <c r="H16" s="8">
+      <c r="H16" s="7">
         <v>161493.20000000001</v>
       </c>
-      <c r="I16" s="8">
+      <c r="I16" s="7">
         <v>77006.240000000005</v>
       </c>
-      <c r="J16" s="13">
+      <c r="J16" s="8">
         <v>29323.240000000002</v>
       </c>
-      <c r="K16" s="13">
+      <c r="K16" s="8">
         <v>191611.01000000001</v>
       </c>
-      <c r="L16" s="13">
+      <c r="L16" s="8">
         <v>210138.81</v>
       </c>
-      <c r="M16" s="14">
+      <c r="M16" s="17">
         <v>2249559.8099999996</v>
       </c>
     </row>
@@ -2324,40 +3380,40 @@
       <c r="A17" s="9">
         <v>44146</v>
       </c>
-      <c r="B17" s="15">
+      <c r="B17" s="12">
         <v>1003723.6899999999</v>
       </c>
-      <c r="C17" s="12">
+      <c r="C17" s="11">
         <v>83071.479999999996</v>
       </c>
-      <c r="D17" s="15">
+      <c r="D17" s="12">
         <v>25329.400000000001</v>
       </c>
-      <c r="E17" s="12">
+      <c r="E17" s="11">
         <v>336918.02000000002</v>
       </c>
-      <c r="F17" s="12">
+      <c r="F17" s="11">
         <v>152899.78</v>
       </c>
-      <c r="G17" s="15">
+      <c r="G17" s="12">
         <v>9596.5300000000007</v>
       </c>
-      <c r="H17" s="12">
+      <c r="H17" s="11">
         <v>167989.29999999999</v>
       </c>
-      <c r="I17" s="12">
+      <c r="I17" s="11">
         <v>77113.860000000001</v>
       </c>
-      <c r="J17" s="15">
+      <c r="J17" s="12">
         <v>29227.389999999999</v>
       </c>
-      <c r="K17" s="15">
+      <c r="K17" s="12">
         <v>192117.12</v>
       </c>
-      <c r="L17" s="15">
+      <c r="L17" s="12">
         <v>210282.97</v>
       </c>
-      <c r="M17" s="16">
+      <c r="M17" s="18">
         <v>2288269.54</v>
       </c>
     </row>
@@ -2365,40 +3421,40 @@
       <c r="A18" s="5">
         <v>44147</v>
       </c>
-      <c r="B18" s="13">
+      <c r="B18" s="8">
         <v>1011544.33</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C18" s="7">
         <v>82322.940000000002</v>
       </c>
-      <c r="D18" s="13">
+      <c r="D18" s="8">
         <v>25085.959999999999</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E18" s="7">
         <v>344544.06</v>
       </c>
-      <c r="F18" s="8">
+      <c r="F18" s="7">
         <v>152213.85999999999</v>
       </c>
-      <c r="G18" s="13">
+      <c r="G18" s="8">
         <v>10554.65</v>
       </c>
-      <c r="H18" s="8">
+      <c r="H18" s="7">
         <v>168738.89999999999</v>
       </c>
-      <c r="I18" s="8">
+      <c r="I18" s="7">
         <v>76949.470000000001</v>
       </c>
-      <c r="J18" s="13">
+      <c r="J18" s="8">
         <v>29104.849999999999</v>
       </c>
-      <c r="K18" s="13">
+      <c r="K18" s="8">
         <v>191995.70999999999</v>
       </c>
-      <c r="L18" s="13">
+      <c r="L18" s="8">
         <v>209709.98000000001</v>
       </c>
-      <c r="M18" s="14">
+      <c r="M18" s="17">
         <v>2302764.71</v>
       </c>
     </row>

</xml_diff>